<commit_message>
deleted duplicate file rna 12.13.19, added biosample and rna sheets for llibrary 5b
</commit_message>
<xml_diff>
--- a/library/Library_hbrown_01.06.20.xlsx
+++ b/library/Library_hbrown_01.06.20.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/library/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01DF3A84-B40B-624D-9459-228F3BDEECE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D65CA56-722B-2C41-9605-E443A1A343FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3580" yWindow="2560" windowWidth="27240" windowHeight="16440" xr2:uid="{4E46FAC1-EF89-5249-852C-DA526C530458}"/>
+    <workbookView xWindow="15860" yWindow="4320" windowWidth="20460" windowHeight="16440" xr2:uid="{4E46FAC1-EF89-5249-852C-DA526C530458}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" iterateDelta="1E-4"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -620,7 +620,7 @@
     <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="61" customWidth="1"/>
+    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>